<commit_message>
Added the refactored codes - now full fledged parallel testing is done
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Ecommerce_WebSite\Ecommerce_WebAutomation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AC02C7-FFF0-4E96-B32C-501558249805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7272D0D1-977C-47B2-884E-B7C4FC352535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{54B80517-B6D3-4988-9698-4D656ACAC352}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -43,35 +43,37 @@
     <t>Password</t>
   </si>
   <si>
-    <t>user1@test</t>
-  </si>
-  <si>
-    <t>user2@test</t>
-  </si>
-  <si>
-    <t>pass123</t>
-  </si>
-  <si>
-    <t>pass456</t>
-  </si>
-  <si>
-    <t>bad1</t>
-  </si>
-  <si>
-    <t>bad2</t>
-  </si>
-  <si>
     <t>short</t>
+  </si>
+  <si>
+    <t>testautomationram@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@1234</t>
+  </si>
+  <si>
+    <t>bad1@gmail.com</t>
+  </si>
+  <si>
+    <t>bad2@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,13 +96,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61685022-3CBD-4768-96C3-697BFD1F81DF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -434,22 +439,18 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F6CF6A21-D86A-485B-8385-F284855AA728}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{39298183-9F97-4C8C-A4DF-00EB722C234F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -459,7 +460,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,22 +478,26 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CBEFFF01-3536-4CE8-B1C2-4A615AF3A959}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{7D991820-8225-4554-BE16-A5FEA8E8A5C9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>